<commit_message>
Added account loading and lookup tables for account to ledgers.
</commit_message>
<xml_diff>
--- a/Ledgers/Andre_Master.xlsx
+++ b/Ledgers/Andre_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\Golang Personal Finance\Ledgers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D469014-4744-4458-87C0-7F0AE78B038F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C9A0A8-BB5F-433E-A55C-1671291000CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Start Balance</t>
   </si>
@@ -38,11 +38,17 @@
   <si>
     <t>Credit Total</t>
   </si>
+  <si>
+    <t>Lookup</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,17 +375,25 @@
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>